<commit_message>
Bugfixes to numeric tolerance test.
</commit_message>
<xml_diff>
--- a/tests/test_artifacts/test_compare_rule_numeric_tolerance/test.xlsx
+++ b/tests/test_artifacts/test_compare_rule_numeric_tolerance/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\i-beg-to-differ\tests\test_artifacts\test_core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\i-beg-to-differ\tests\test_artifacts\test_compare_rule_numeric_tolerance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5CE4A4-02B0-4EED-A56B-483C4F075D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33FF384-CE3E-4CDB-B62A-0D268A5B530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7104" yWindow="2424" windowWidth="23040" windowHeight="12660" xr2:uid="{E0987C40-DE28-48BA-BC2C-209A11D1EF12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{E0987C40-DE28-48BA-BC2C-209A11D1EF12}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,10 +526,10 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="E2">
-        <v>7.4127384735807968</v>
+        <v>7.4210632309999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -546,7 +546,7 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>3.1097419535443795</v>
+        <v>3.1039137929999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -560,10 +560,10 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>9.25</v>
       </c>
       <c r="E4">
-        <v>10.497180630266294</v>
+        <v>10.504359301999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -577,10 +577,10 @@
         <v>28</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="E5">
-        <v>7.9065868521777345</v>
+        <v>7.9139052420000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -594,10 +594,10 @@
         <v>29</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>9.25</v>
       </c>
       <c r="E6">
-        <v>8.2886376058927969</v>
+        <v>8.2814382280000007</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -614,7 +614,7 @@
         <v>6</v>
       </c>
       <c r="E7">
-        <v>10.457065481556475</v>
+        <v>10.461241478</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -628,10 +628,10 @@
         <v>31</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="E8">
-        <v>3.8482210167506947</v>
+        <v>3.844897413</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>0.33985071739382744</v>
+        <v>0.32989912399999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -662,10 +662,10 @@
         <v>33</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="E10">
-        <v>8.2641600064017613</v>
+        <v>8.2660064749999993</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -679,10 +679,10 @@
         <v>34</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="E11">
-        <v>8.1822368578921321</v>
+        <v>8.1876301999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>